<commit_message>
Added feature. Look up alternative name for unfound company
</commit_message>
<xml_diff>
--- a/companies.xlsx
+++ b/companies.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t xml:space="preserve">Company name</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">Specialties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LinkedIn</t>
   </si>
   <si>
     <t xml:space="preserve">ADORSYS</t>
@@ -553,8 +556,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -566,7 +569,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="27.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="30"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="27.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="11.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="11.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="23.08"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="11" style="1" width="10.83"/>
   </cols>
@@ -602,13 +605,16 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" s="4" customFormat="true" ht="412.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="1"/>
@@ -622,447 +628,447 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>